<commit_message>
Topo and BA added
</commit_message>
<xml_diff>
--- a/examples/data/jwgrav.xlsx
+++ b/examples/data/jwgrav.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/ab14785_bristol_ac_uk/Documents/01-Coding/6-Github_repos/mgravpy/examples/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/ab14785_bristol_ac_uk/Documents/01-Coding/6-Github_repos/mugravpy/examples/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_65FF4FDB7CB7B36EBD9BA0016728893B53D8EC2F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0467AF1-615E-BC48-ADBD-51C83E3C153F}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_65FF4FDB7CB7B36EBD9BA0016728893B53D8EC2F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98DADB06-D8E7-7A4F-9593-2AD1D32D0497}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="580" windowWidth="51200" windowHeight="20600" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52300" yWindow="1820" windowWidth="32980" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Line 1" sheetId="1" r:id="rId1"/>
@@ -4042,8 +4042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10218,7 +10218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>

</xml_diff>